<commit_message>
added new room and tests
</commit_message>
<xml_diff>
--- a/Clue_LayoutStudent.xlsx
+++ b/Clue_LayoutStudent.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="24">
   <si>
     <t>w</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>PR</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>JL</t>
   </si>
 </sst>
 </file>
@@ -97,7 +103,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -128,6 +134,54 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0066"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -141,12 +195,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,7 +511,7 @@
   <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z26" sqref="Z26"/>
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -496,7 +558,7 @@
       <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -514,7 +576,7 @@
       <c r="N1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="P1" s="2" t="s">
@@ -777,7 +839,7 @@
       <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -792,7 +854,7 @@
       <c r="H5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="8" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
@@ -878,7 +940,7 @@
       <c r="L6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="6" t="s">
         <v>0</v>
       </c>
       <c r="N6" s="1" t="s">
@@ -922,7 +984,7 @@
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -967,7 +1029,7 @@
       <c r="Q7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="R7" s="4" t="s">
+      <c r="R7" s="10" t="s">
         <v>14</v>
       </c>
       <c r="S7" s="2" t="s">
@@ -1056,7 +1118,7 @@
       <c r="V8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="W8" s="1" t="s">
+      <c r="W8" s="5" t="s">
         <v>0</v>
       </c>
       <c r="X8">
@@ -1121,14 +1183,14 @@
       <c r="S9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="U9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="V9" s="2" t="s">
-        <v>17</v>
+      <c r="T9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W9" s="1" t="s">
         <v>0</v>
@@ -1195,17 +1257,17 @@
       <c r="S10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T10" s="2" t="s">
-        <v>17</v>
+      <c r="T10" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="X10">
         <v>9</v>
@@ -1233,7 +1295,7 @@
       <c r="G11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="11" t="s">
         <v>0</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -1269,17 +1331,17 @@
       <c r="S11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T11" s="2" t="s">
-        <v>17</v>
+      <c r="T11" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="X11">
         <v>10</v>
@@ -1328,7 +1390,7 @@
       <c r="N12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="O12" s="8" t="s">
         <v>0</v>
       </c>
       <c r="P12" s="4" t="s">
@@ -1343,17 +1405,17 @@
       <c r="S12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>17</v>
+      <c r="T12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U12" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="X12">
         <v>11</v>
@@ -1417,17 +1479,17 @@
       <c r="S13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="U13" s="2" t="s">
-        <v>17</v>
+      <c r="T13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U13" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="X13">
         <v>12</v>
@@ -1446,7 +1508,7 @@
       <c r="D14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -1491,24 +1553,24 @@
       <c r="S14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T14" s="2" t="s">
-        <v>17</v>
+      <c r="T14" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="X14">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:24">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1526,7 +1588,7 @@
       <c r="F15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="6" t="s">
         <v>0</v>
       </c>
       <c r="H15" s="1" t="s">
@@ -1565,17 +1627,17 @@
       <c r="S15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T15" s="2" t="s">
-        <v>17</v>
+      <c r="T15" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="X15">
         <v>14</v>
@@ -1639,14 +1701,14 @@
       <c r="S16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="T16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="U16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="V16" s="2" t="s">
-        <v>17</v>
+      <c r="T16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W16" s="1" t="s">
         <v>0</v>
@@ -1665,7 +1727,7 @@
       <c r="C17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -1701,7 +1763,7 @@
       <c r="O17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="P17" s="12" t="s">
         <v>0</v>
       </c>
       <c r="Q17" s="1" t="s">
@@ -1710,7 +1772,7 @@
       <c r="R17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="S17" s="1" t="s">
+      <c r="S17" s="9" t="s">
         <v>0</v>
       </c>
       <c r="T17" s="1" t="s">
@@ -1751,7 +1813,7 @@
       <c r="G18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="11" t="s">
         <v>0</v>
       </c>
       <c r="I18" s="1" t="s">
@@ -1763,7 +1825,7 @@
       <c r="K18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="L18" s="8" t="s">
         <v>0</v>
       </c>
       <c r="M18" s="1" t="s">
@@ -1858,7 +1920,7 @@
       <c r="R19" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S19" s="4" t="s">
+      <c r="S19" s="7" t="s">
         <v>16</v>
       </c>
       <c r="T19" s="2" t="s">
@@ -2047,7 +2109,7 @@
       <c r="G22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I22" s="1" t="s">
@@ -2068,7 +2130,7 @@
       <c r="N22" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="O22" s="1" t="s">
+      <c r="O22" s="5" t="s">
         <v>0</v>
       </c>
       <c r="P22" s="2" t="s">

</xml_diff>

<commit_message>
Refactorization: itialize no longer hardcoded
</commit_message>
<xml_diff>
--- a/Clue_LayoutStudent.xlsx
+++ b/Clue_LayoutStudent.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
@@ -18,9 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="24">
   <si>
-    <t>w</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -88,13 +85,16 @@
   </si>
   <si>
     <t>JL</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,6 +298,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -332,6 +333,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -507,14 +509,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="3.42578125" bestFit="1" customWidth="1"/>
@@ -533,1635 +535,1635 @@
     <col min="22" max="24" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="O5" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R7" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="W8" s="5" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="X8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="R9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S9" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="T9" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="X9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="X10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="X11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="U12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="X12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="U13" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="X13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="X14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="X15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="X16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P17" s="12" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="S17" s="9" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="X17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="X18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q19" s="2" t="s">
+      <c r="S19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="R19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="S19" s="7" t="s">
-        <v>16</v>
-      </c>
       <c r="T19" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="W20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="W21" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V22" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:24">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -2238,24 +2240,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>